<commit_message>
SD Card logging added
</commit_message>
<xml_diff>
--- a/Stack_Heap_calcs.xlsx
+++ b/Stack_Heap_calcs.xlsx
@@ -419,7 +419,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,12 +525,12 @@
         <v>103360</v>
       </c>
       <c r="N2" s="2">
-        <f>8*15360</f>
-        <v>122880</v>
+        <f>7.5*15360</f>
+        <v>115200</v>
       </c>
       <c r="O2" s="2">
         <f>N2-M2</f>
-        <v>19520</v>
+        <v>11840</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -586,11 +586,11 @@
       </c>
       <c r="N3" s="2">
         <f>N2/1024</f>
-        <v>120</v>
+        <v>112.5</v>
       </c>
       <c r="O3" s="2">
         <f>O2/1024</f>
-        <v>19.0625</v>
+        <v>11.5625</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
system's memory monitoring added(free stacks & heap) corrected publishLog function
</commit_message>
<xml_diff>
--- a/Stack_Heap_calcs.xlsx
+++ b/Stack_Heap_calcs.xlsx
@@ -38,18 +38,6 @@
     <t>RAM</t>
   </si>
   <si>
-    <t>Stack1</t>
-  </si>
-  <si>
-    <t>Stack2</t>
-  </si>
-  <si>
-    <t>Stack3</t>
-  </si>
-  <si>
-    <t>Stack4</t>
-  </si>
-  <si>
     <t>Stack5</t>
   </si>
   <si>
@@ -72,6 +60,18 @@
   </si>
   <si>
     <t>uint32_t 1-byte dynamic queue on Heap</t>
+  </si>
+  <si>
+    <t>Stack2 - SDCard</t>
+  </si>
+  <si>
+    <t>Stack1 - SysMon</t>
+  </si>
+  <si>
+    <t>Stack3 - WlsCom</t>
+  </si>
+  <si>
+    <t>Stack4 - IrrCtrl</t>
   </si>
 </sst>
 </file>
@@ -419,13 +419,17 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.109375" customWidth="1"/>
     <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
     <col min="12" max="12" width="12.109375" customWidth="1"/>
     <col min="13" max="13" width="10.109375" customWidth="1"/>
     <col min="14" max="14" width="13.44140625" customWidth="1"/>
@@ -434,31 +438,31 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
@@ -467,13 +471,13 @@
         <v>3</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -488,12 +492,12 @@
         <v>112</v>
       </c>
       <c r="D2" s="2">
-        <f>B2+C2</f>
-        <v>624</v>
+        <f>30*B2+C2</f>
+        <v>15472</v>
       </c>
       <c r="E2" s="2">
-        <f>120*B2+C2</f>
-        <v>61552</v>
+        <f>80*B2+C2</f>
+        <v>41072</v>
       </c>
       <c r="F2" s="2">
         <f>20*B2+C2</f>
@@ -522,7 +526,7 @@
       </c>
       <c r="M2" s="2">
         <f>SUM(D2:I2)</f>
-        <v>103360</v>
+        <v>97728</v>
       </c>
       <c r="N2" s="2">
         <f>7.5*15360</f>
@@ -530,7 +534,7 @@
       </c>
       <c r="O2" s="2">
         <f>N2-M2</f>
-        <v>11840</v>
+        <v>17472</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -547,11 +551,11 @@
       </c>
       <c r="D3" s="2">
         <f>D2/1024</f>
-        <v>0.609375</v>
+        <v>15.109375</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:H3" si="0">E2/1024</f>
-        <v>60.109375</v>
+        <v>40.109375</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" si="0"/>
@@ -582,7 +586,7 @@
       </c>
       <c r="M3" s="2">
         <f>SUM(D3:I3)</f>
-        <v>100.9375</v>
+        <v>95.4375</v>
       </c>
       <c r="N3" s="2">
         <f>N2/1024</f>
@@ -590,13 +594,13 @@
       </c>
       <c r="O3" s="2">
         <f>O2/1024</f>
-        <v>11.5625</v>
+        <v>17.0625</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>

</xml_diff>